<commit_message>
examples: add PEP GDP SAM comparison and update CRI reference data
</commit_message>
<xml_diff>
--- a/src/equilibria/templates/reference/pep2/data/SAM-CRI-gams-fixed.xlsx
+++ b/src/equilibria/templates/reference/pep2/data/SAM-CRI-gams-fixed.xlsx
@@ -999,7 +999,7 @@
         <v>1699909.001579771</v>
       </c>
       <c r="K7" t="n">
-        <v>2508494.69219632</v>
+        <v>1664389.427118422</v>
       </c>
       <c r="L7" t="n">
         <v>938917.9349794999</v>
@@ -1007,6 +1007,18 @@
       <c r="M7" t="n">
         <v>10044.5766143</v>
       </c>
+      <c r="S7" t="n">
+        <v>42609.24106857165</v>
+      </c>
+      <c r="T7" t="n">
+        <v>40977.06289665159</v>
+      </c>
+      <c r="U7" t="n">
+        <v>297477.3920892276</v>
+      </c>
+      <c r="V7" t="n">
+        <v>463041.5690234468</v>
+      </c>
       <c r="W7" t="n">
         <v>120748.2386780651</v>
       </c>
@@ -1240,18 +1252,6 @@
       </c>
       <c r="R14" t="n">
         <v>408327.9979946495</v>
-      </c>
-      <c r="S14" t="n">
-        <v>42609.24106857165</v>
-      </c>
-      <c r="T14" t="n">
-        <v>40977.06289665159</v>
-      </c>
-      <c r="U14" t="n">
-        <v>297477.3920892276</v>
-      </c>
-      <c r="V14" t="n">
-        <v>463041.5690234468</v>
       </c>
     </row>
     <row r="15">

</xml_diff>